<commit_message>
adding some datasets from powerBI and SMOTE for machine learning
</commit_message>
<xml_diff>
--- a/data science.xlsx
+++ b/data science.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aditya\Downloads-D\Data Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9362C211-128C-4B30-B516-38A258A8B70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E99B35-118D-4389-B79A-981735B8267E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{069A844D-913F-4D34-8028-C0CA24D2AD78}"/>
   </bookViews>
@@ -4414,7 +4414,7 @@
   <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4513,7 +4513,7 @@
         <v>173</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>